<commit_message>
Add Upwind and OptiMat
</commit_message>
<xml_diff>
--- a/output/material_split.xlsx
+++ b/output/material_split.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MD-SLC-UP3-V(±45/0/±45/0/±45)</t>
+          <t>MD-SLA-UP3-V(±45/0/±45/0/±45)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UNI-A060-UP2[0]10</t>
+          <t>UNI-A[0]5</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MD-TLT1200-EP5-D(±45/(0)2)S</t>
+          <t>MD-SLB-UP3-V(±45/0/±45/0/±45)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>UNI-A130C-UP2[0]6</t>
+          <t>UNI-B[0]5</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MD-TT-EP3-V(±45/0/±45/0/±45)</t>
+          <t>MD-SLC-UP3-V(±45/0/±45/0/±45)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>UNI-A130G-UP2[0]6</t>
+          <t>UNI-CA-VE2[0]12</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MD-TT1A-EP1-V(±45/0/±45/0/±45)</t>
+          <t>MD-TLT1200-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>UNI-A260-UP2[0]4</t>
+          <t>UNI-CM1701A-UP2[0]5</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MD-TT2-EP1-V(±45/0/0/0/±45)</t>
+          <t>MD-TT-EP3-V(±45/0/±45/0/±45)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>UNI-AGY S1HM-EP1[0]2</t>
+          <t>UNI-D072A-UP2[0]10</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MD-TT5-EP1-P((±45)2/(0)2)S</t>
+          <t>MD-TT1A-EP1-V(±45/0/±45/0/±45)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>UNI-A[0]5</t>
+          <t>UNI-D092B-UP2[0]9</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MD-TT7-EP1-V(±45/0/±45/0/±45)</t>
+          <t>MD-TT2-EP1-V(±45/0/0/0/±45)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>UNI-B[0]5</t>
+          <t>UNI-D092D-UP2[0]7</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MD-WS1-EP5(±45/0/±45)</t>
+          <t>MD-TT5-EP1-P((±45)2/(0)2)S</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>UNI-CA-VE2[0]12</t>
+          <t>UNI-D092F-UP2[0]12</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MD-X[(0)2/M/±45/(0)2)]</t>
+          <t>MD-TT7-EP1-V(±45/0/±45/0/±45)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UNI-CM1701A-UP2[0]5</t>
+          <t>UNI-D092G-UP2[0]14</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MD-X[(90)2/M/±45/(90)2)]</t>
+          <t>MD-WS1-EP5(±45/0/±45)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>UNI-D072A-UP2[0]10</t>
+          <t>UNI-D155B-UP2[0]5</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MD-Y[(0)2/M/±45/(0)2)]</t>
+          <t>MD-X[(0)2/M/±45/(0)2)]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>UNI-D092B-UP2[0]9</t>
+          <t>UNI-D155C-UP2[0]7</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>N1[0b]2S</t>
+          <t>MD-X[(90)2/M/±45/(90)2)]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>UNI-D092D-UP2[0]7</t>
+          <t>UNI-D155C2-UP2[0]7</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P10[0]6</t>
+          <t>MD-Y[(0)2/M/±45/(0)2)]</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>UNI-D092F-UP2[0]12</t>
+          <t>UNI-D155G-UP2[0]8</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P11[0/90]3</t>
+          <t>ROV2-UP2[0/90]4</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>UNI-D092G-UP2[0]14</t>
+          <t>UNI-D155H-UP2[0]7</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P12[0]6</t>
+          <t>ROV3-UP2[0/90]5</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>UNI-D155B-UP2[0]5</t>
+          <t>UNI-D155J-UP2[0]9</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P13[0/90]3</t>
+          <t>ROV4-UP4[0/90]8</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>UNI-D155C-UP2[0]7</t>
+          <t>UNI-D155K-UP2[0]7</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P14[0]6</t>
+          <t>TRIAX-OC1800-EP1(±45/0)(±45/0)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>UNI-D155C2-UP2[0]7</t>
+          <t>UNI-ELT5500-EP1[0]2</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P1[0/90]3</t>
+          <t>TRIAX-OC1800-EP1(±45/0)S</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>UNI-D155G-UP2[0]8</t>
+          <t>UNI-ELT5500-EP1[0]6</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P2[0]6</t>
+          <t>TRIAX-S1200-EP1(±45/0)S</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>UNI-D155H-UP2[0]7</t>
+          <t>UNI-ELT5500-UP5[0]2</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P3[0]6</t>
+          <t>TRIAX-S800-EP1(±45/0)S</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>UNI-D155J-UP2[0]9</t>
+          <t>UNI-ELT5500-VE4[0]2</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4[0/90]3</t>
+          <t>Triax-AA-UP2[(±45/0)3/(0/±45)2]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>UNI-D155K-UP2[0]7</t>
+          <t>UNI-L[0]3</t>
         </is>
       </c>
     </row>
@@ -815,542 +815,474 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P5[0/90]3</t>
+          <t>Triax-AA3-UP2[(±45/0)3]S</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>UNI-ELT5500-EP1[0]2</t>
+          <t>UNI-MM1(0)N</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>C32/C33(0/90)5</t>
+          <t>Carbon prepreg[0]2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P6[0/90]3</t>
+          <t>Triax-AA4-UP2[(±45/0)2]S</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>UNI-ELT5500-EP1[0]6</t>
+          <t>UNI-MM2(0)N</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>C34/C35(0/90)5</t>
+          <t>Carbon prepreg[±45/[0]2/±45]</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P7[0]6</t>
+          <t>Triax-DD27A-UP2[0/±45]S</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>UNI-ELT5500-UP5[0]2</t>
+          <t>UNI-Neptco Rodpack[0]2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>C36/C37(0/90)5</t>
+          <t>DB-BIAX-DE2[(+/-45)S]3</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8[0]6</t>
+          <t>Triax-DD27B-UP2[0/±45]S</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>UNI-ELT5500-VE4[0]2</t>
+          <t>UNI-Neptco Rodpack[0]4</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>C38/C39(0/90)9</t>
+          <t>DB-BIAX-DE4[(+/-45)S]3</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P9[0/90]3</t>
+          <t>Triax-H[(±45/0)3]S</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>UNI-L[0]3</t>
+          <t>UNI-OCV1000-EP1[0]2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CE1[V(+/-45)g/0c]S</t>
+          <t>DB-BIAX-FGI1708-EP1(RM/±45)3S</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ROV2-UP2[0/90]4</t>
+          <t>Triax-J[(0/±45)3]S</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>UNI-MM1(0)N</t>
+          <t>UNI-OCV1200-EP1[0]2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CE2[V(+/-45)g/0c]S</t>
+          <t>DB-BIAX-FGI1708-UP1(RM/±45)3S</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ROV3-UP2[0/90]5</t>
+          <t>Triax-M[(0/±45)4]</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>UNI-MM2(0)N</t>
+          <t>UNI-OCV1322-EP1[0]2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CE3[V(+/-45)g/0c]S</t>
+          <t>DB-BIAX-SWA-EP1(±45)6</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ROV4-UP4[0/90]8</t>
+          <t>Triax-N[(0/±45)4]</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>UNI-Neptco Rodpack[0]2</t>
+          <t>UNI-PPG1200-EP1[0]2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CE4[V(+/-45)g/0c]S</t>
+          <t>EP1 Neat Resin Neat Resin</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TRIAX-OC1800-EP1(±45/0)(±45/0)</t>
+          <t>Triax-N[(90/±45)4]</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>UNI-Neptco Rodpack[0]4</t>
+          <t>UNI-PPG1200-EP5[90]4</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CE5[V(+/-45)g/0c]S</t>
+          <t>LCCF-K20[0]5</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TRIAX-OC1800-EP1(±45/0)S</t>
+          <t>Triax-R[0/±45]4</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>UNI-OCV1000-EP1[0]2</t>
+          <t>UNI-PPG1200-PU[0]6</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CE6[V/0/45/-45/0/V]</t>
+          <t>LCCF-T20[0]5</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TRIAX-S1200-EP1(±45/0)S</t>
+          <t>Triax-T[(0/±45)5]</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>UNI-OCV1200-EP1[0]2</t>
+          <t>UNI-PPG1200-UP5[0]2</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Carbon prepreg(0)2</t>
+          <t>MD-10D155-UP2[±10]3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TRIAX-S800-EP1(±45/0)S</t>
+          <t>Triax-U[(0/±45)5]</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>UNI-OCV1322-EP1[0]2</t>
+          <t>UNI-PPG1200-VE2[0]2</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Carbon prepreg[0]2</t>
+          <t>MD-20D155-UP2[±20]3</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Triax-AA-UP2[(±45/0)3/(0/±45)2]</t>
+          <t>Triax-V[(0/±45)5]</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>UNI-PPG1200-EP1[0]2</t>
+          <t>UNI-PPG1200-VE4[0]2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Carbon prepreg[±45/[0]2/±45]</t>
+          <t>MD-30D155-UP2[±30]3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Triax-AA3-UP2[(±45/0)3]S</t>
+          <t>UNI-(0)2-UP2[0]2</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>UNI-PPG1200-EP5[90]4</t>
+          <t>UNI-PPG1250-EP1[0]2</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Carbon/glass hybrid prepregs(±45/(0)2/±45)</t>
+          <t>MD-40D155-UP2[±40]3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Triax-AA4-UP2[(±45/0)2]S</t>
+          <t>UNI-(90)4-UP2[90]4</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>UNI-PPG1200-PU[0]6</t>
+          <t>UNI-PPG1250-EP5[0]2</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DB-BIAX-DE2[(+/-45)S]3</t>
+          <t>MD-45D155-UP2[±45]3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Triax-DD27A-UP2[0/±45]S</t>
+          <t>UNI-90D155E2-SC14[90]6</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>UNI-PPG1200-UP5[0]2</t>
+          <t>UNI-PPGHYBON2400-EP5[0]4</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>DB-BIAX-DE4[(+/-45)S]3</t>
+          <t>MD-45D155P2-UP4[±45]3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Triax-DD27B-UP2[0/±45]S</t>
+          <t>UNI-90D155V-VE[90]6</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>UNI-PPG1200-VE2[0]2</t>
+          <t>UNI-PPGHYBON2400-UP5[0]4</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>DB-BIAX-DH3-EP1(+/-45)6</t>
+          <t>MD-45D155V-VE[±45]3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Triax-H[(±45/0)3]S</t>
+          <t>UNI-90D155V2-VE2[90]6</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>UNI-PPG1200-VE4[0]2</t>
+          <t>UNI-PPGHYBON2400-VE4[0]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DB-BIAX-FGI1708-EP1(RM/±45)3S</t>
+          <t>MD-50D155-UP2[±50]3</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Triax-J[(0/±45)3]S</t>
+          <t>UNI-A060-UP2[0]10</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>UNI-PPG1250-EP1(0)2</t>
+          <t>UNI-PPGHYBON2400-VE5[0]4</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DB-BIAX-FGI1708-UP1(RM/±45)3S</t>
+          <t>MD-60D155-UP2[±60]3</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Triax-M[(0/±45)4]</t>
+          <t>UNI-A130C-UP2[0]6</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>UNI-PPG1250-EP10(0)2</t>
+          <t>UNI-PPGHYBON2400-VE6[0]4</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>DB-BIAX-SWA-EP1(±45)6</t>
+          <t>MD-70D155-UP2[±70]3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Triax-N[(0/±45)4]</t>
+          <t>UNI-A130G-UP2[0]6</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>UNI-PPG1250-EP1[0]2</t>
+          <t>UNI-PPGHYBON4400-VE4[0]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>EP1 Neat Resin Neat Resin</t>
+          <t>MD-80D155-UP2[±80]3</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Triax-N[(90/±45)4]</t>
+          <t>UNI-A260-UP2[0]4</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>UNI-PPG1250-EP5[0]2</t>
+          <t>UNI-UNI21-VE2[0]4</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>J1[0/45/90/-45]4</t>
+          <t>MD-90D155-UP2[90]6</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Triax-R[0/±45]4</t>
+          <t>UNI-AGY S1HM-EP1[0]2</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>UNI-PPG1250-EP9(0)2</t>
+          <t>UNI-UNI25-VE2[0]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>J2[0/45/90/-45]4</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Triax-T[(0/±45)5]</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>UNI-PPG1250-VE7(0)2</t>
-        </is>
-      </c>
+          <t>MD-BB-UP2[±45/(0)2/+45]S</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>J3[0/45/90/-45]4</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Triax-U[(0/±45)5]</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>UNI-PPGHYBON2400-EP5[0]4</t>
-        </is>
-      </c>
+          <t>MD-BB-UP2[±45/(90)2/+45]S</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>J4[(0/90)(45/-45)]4</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Triax-V[(0/±45)5]</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>UNI-PPGHYBON2400-UP5[0]4</t>
-        </is>
-      </c>
+          <t>MD-CC-UP2[±45/(0)2/+45]S</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>J5[(0/90)(45/-45)]4</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>UNI-(0)2-UP2[0]2</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>UNI-PPGHYBON2400-VE4[0]</t>
-        </is>
-      </c>
+          <t>MD-CC2-UP2[±45/(0)3/+45]S</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>J6[(0/90)(45/-45)]4</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>UNI-(90)4-UP2[90]4</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>UNI-PPGHYBON2400-VE5[0]4</t>
-        </is>
-      </c>
+          <t>MD-CC3-UP2[0/±45/(0)2/+45]S</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>J7[0/45/90/-45]8</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>UNI-90D155E2-SC14[90]6</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>UNI-PPGHYBON2400-VE6[0]4</t>
-        </is>
-      </c>
+          <t>MD-CYC[(±45)2/(0)10]S</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>J8[(0/90)(45/-45)]4</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>UNI-90D155V-VE[90]6</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>UNI-PPGHYBON4400-VE4[0]</t>
-        </is>
-      </c>
+          <t>MD-DD-UP2[0/±45/(0)3/±45/0]</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LCCF-K20[0]5</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>UNI-90D155V2-VE2[90]6</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>UNI-UNI21-VE2[0]4</t>
-        </is>
-      </c>
+          <t>MD-DD10-UP2[0/±45/0]S</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>LCCF-T20[0]5</t>
+          <t>MD-DD11-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>UNI-UNI25-VE2[0]</t>
-        </is>
-      </c>
+      <c r="C54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>MD-10D155-UP2[±10]3</t>
+          <t>MD-DD11-UP2[90/±45/90]S</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1359,7 +1291,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>MD-20D155-UP2[±20]3</t>
+          <t>MD-DD11E3-EP3[0/±45/0]S</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1368,7 +1300,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MD-30D155-UP2[±30]3</t>
+          <t>MD-DD12-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1377,7 +1309,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MD-40D155-UP2[±40]3</t>
+          <t>MD-DD13-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1386,7 +1318,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MD-45D155-UP2[±45]3</t>
+          <t>MD-DD14-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1395,7 +1327,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MD-45D155P2-UP4[±45]3</t>
+          <t>MD-DD18-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1404,7 +1336,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MD-45D155V-VE[±45]3</t>
+          <t>MD-DD18A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1413,7 +1345,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MD-50D155-UP2[±50]3</t>
+          <t>MD-DD19-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1422,7 +1354,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>MD-60D155-UP2[±60]3</t>
+          <t>MD-DD19A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1431,7 +1363,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MD-70D155-UP2[±70]3</t>
+          <t>MD-DD19A-UP2[90/±45/90]S</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1440,7 +1372,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>MD-80D155-UP2[±80]3</t>
+          <t>MD-DD19B-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1449,7 +1381,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MD-90D155-UP2[90]6</t>
+          <t>MD-DD2-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1458,7 +1390,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MD-BB-UP2[±45/(0)2/+45]S</t>
+          <t>MD-DD20-UP2[(0)2/±45/0]S</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1467,7 +1399,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MD-BB-UP2[±45/(90)2/+45]S</t>
+          <t>MD-DD20A-UP2[(0)2/±45/0]S</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1476,7 +1408,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MD-CC-UP2[±45/(0)2/+45]S</t>
+          <t>MD-DD22-UP2[(0)2/±45/0]S</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -1485,7 +1417,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MD-CC2-UP2[±45/(0)3/+45]S</t>
+          <t>MD-DD24-UP2[0/±45/(0)3/±45/0]</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1494,7 +1426,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MD-CC3-UP2[0/±45/(0)2/+45]S</t>
+          <t>MD-DD25-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -1503,7 +1435,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>MD-CYC[(±45)2/(0)10]S</t>
+          <t>MD-DD25A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1512,7 +1444,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MD-DD-UP2[0/±45/(0)3/±45/0]</t>
+          <t>MD-DD25B-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -1521,7 +1453,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MD-DD10-UP2[0/±45/0]S</t>
+          <t>MD-DD26-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -1530,7 +1462,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>MD-DD11-UP2[0/±45/0]S</t>
+          <t>MD-DD2A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -1539,7 +1471,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MD-DD11-UP2[90/±45/90]S</t>
+          <t>MD-DD4-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -1548,7 +1480,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MD-DD11E3-EP3[0/±45/0]S</t>
+          <t>MD-DD5-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -1557,7 +1489,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>MD-DD12-UP2[0/±45/0]S</t>
+          <t>MD-DD5CYC-T[0/±45/0]S</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -1566,7 +1498,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>MD-DD13-UP2[0/±45/0]S</t>
+          <t>MD-DD5E-Epon9410[0/±45/0]S</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -1575,7 +1507,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>MD-DD14-UP2[0/±45/0]S</t>
+          <t>MD-DD5E3-EP3[0/±45/0]S</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -1584,7 +1516,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>MD-DD18-UP2[0/±45/0]S</t>
+          <t>MD-DD5P-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -1593,7 +1525,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>MD-DD18A-UP2[0/±45/0]S</t>
+          <t>MD-DD5P-UP2[90/±45/90]S</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -1602,7 +1534,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>MD-DD19-UP2[0/±45/0]S</t>
+          <t>MD-DD5V-VE1[0/±45/0]S</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -1611,7 +1543,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>MD-DD19A-UP2[0/±45/0]S</t>
+          <t>MD-DD5V2-VE2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -1620,7 +1552,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>MD-DD19A-UP2[90/±45/90]S</t>
+          <t>MD-DD5V3-Dion9800[0/±45/0]S</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -1629,7 +1561,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>MD-DD19B-UP2[0/±45/0]S</t>
+          <t>MD-DD6-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -1638,7 +1570,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>MD-DD2-UP2[0/±45/0]S</t>
+          <t>MD-DD7-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -1647,7 +1579,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>MD-DD20-UP2[(0)2/±45/0]S</t>
+          <t>MD-DD8-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -1656,7 +1588,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>MD-DD20A-UP2[(0)2/±45/0]S</t>
+          <t>MD-EEAP[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -1665,7 +1597,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>MD-DD22-UP2[(0)2/±45/0]S</t>
+          <t>MD-EEAV[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -1674,7 +1606,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>MD-DD24-UP2[0/±45/(0)3/±45/0]</t>
+          <t>MD-EEBP[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -1683,7 +1615,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>MD-DD25-UP2[0/±45/0]S</t>
+          <t>MD-EECP[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -1692,7 +1624,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>MD-DD25A-UP2[0/±45/0]S</t>
+          <t>MD-EE[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -1701,7 +1633,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>MD-DD25B-UP2[0/±45/0]S</t>
+          <t>MD-ELT5500-EP4[±45/0/±45/0/±45]</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -1710,7 +1642,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>MD-DD26-UP2[0/±45/0]S</t>
+          <t>MD-ELT5500-VE3[±45/0/±45/0/±45]</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -1719,7 +1651,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>MD-DD2A-UP2[0/±45/0]S</t>
+          <t>MD-FFA-UP2[±45/0/0/±45]S</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -1728,7 +1660,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>MD-DD4-UP2[0/±45/0]S</t>
+          <t>MD-FFB-UP2[0/±45/0/±45/0]S</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -1737,7 +1669,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>MD-DD5-UP2[0/±45/0]S</t>
+          <t>MD-FFC-UP2[0/±45/±45/0]S</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -1746,7 +1678,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>MD-DD5CYC-T[0/±45/0]S</t>
+          <t>MD-FFD-UP2[0/0/±45/±45]S</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -1755,7 +1687,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>MD-DD5E-Epon9410[0/±45/0]S</t>
+          <t>MD-FFF-UP2[±45/±45/0/0]S</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -1764,7 +1696,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>MD-DD5E3-EP3[0/±45/0]S</t>
+          <t>MD-GG-UP2[(0)2/±45/(0)2]</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -1773,7 +1705,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>MD-DD5P-UP2-Enviro[0/±45/0]S</t>
+          <t>MD-GGP2-prepreg[0/±45/0]</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -1782,7 +1714,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>MD-DD5P-UP2[0/±45/0]S</t>
+          <t>MD-GGP4-prepreg[0/±45/0]</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -1791,7 +1723,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>MD-DD5P-UP2[90/±45/90]S</t>
+          <t>MD-HHInjected Short Carbon fiber</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -1800,7 +1732,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>MD-DD5V-VE1[0/±45/0]S</t>
+          <t>MD-Hybrid CG-VE[(0)2/(0)2C/0/(0)2C/(0)2]</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -1809,7 +1741,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>MD-DD5V2-VE2[0/±45/0]S</t>
+          <t>MD-Hybrid CGB-prepreg[(0)2C/±45/(0)2C)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -1818,7 +1750,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>MD-DD5V3-Dion9800[0/±45/0]S</t>
+          <t>MD-Hybrid CGB3-prepreg[(±45G)/(0)3C/(±45G)]</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -1827,7 +1759,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>MD-DD6-UP2[0/±45/0]S</t>
+          <t>MD-Hybrid CGD4-VE2[(±45G)/(0)3C/(±45G)]</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -1836,7 +1768,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>MD-DD7-UP2[0/±45/0]S</t>
+          <t>MD-Hybrid CGD4E-EP3[(±45G)/(0)3C/(±45G)]</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -1845,7 +1777,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>MD-DD8-UP2[0/±45/0]S</t>
+          <t>MD-Hybrid JJ-VE2[(±45)/(0)3C/±45)]</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -1854,7 +1786,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>MD-EEAP[M/±45/0)S]</t>
+          <t>MD-L1200-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -1863,7 +1795,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>MD-EEAV[M/±45/0)S]</t>
+          <t>MD-L1400BTW-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -1872,7 +1804,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>MD-EEBP[M/±45/0)S]</t>
+          <t>MD-L1400T-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -1881,7 +1813,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>MD-EECP[M/±45/0)S]</t>
+          <t>MD-L1400TCS-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -1890,7 +1822,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>MD-EE[M/±45/0)S]</t>
+          <t>MD-L1400TCU-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -1899,7 +1831,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>MD-ELT5500-EP4[±45/0/±45/0/±45]</t>
+          <t>MD-L1400Thru-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -1908,7 +1840,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>MD-ELT5500-VE3[±45/0/±45/0/±45]</t>
+          <t>MD-L2400-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -1917,7 +1849,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>MD-FFA-UP2[±45/0/0/±45]S</t>
+          <t>MD-LT1200-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -1926,7 +1858,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>MD-FFB-UP2[0/±45/0/±45/0]S</t>
+          <t>MD-LT1200G50-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -1935,7 +1867,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>MD-FFC-UP2[0/±45/±45/0]S</t>
+          <t>MD-P2B[±45/(0)4C]S</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -1944,7 +1876,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>MD-FFD-UP2[0/0/±45/±45]S</t>
+          <t>MD-P2B[±45/(90)4C]S</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -1953,7 +1885,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>MD-FFF-UP2[±45/±45/0/0]S</t>
+          <t>MD-P2C[(±45)/(0)4]S</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -1962,7 +1894,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>MD-GG-UP2[(0)2/±45/(0)2]</t>
+          <t>MD-PPG1200-EP1[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -1971,7 +1903,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>MD-GGP2-prepreg[0/±45/0]</t>
+          <t>MD-PPG1200-UP5[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -1980,7 +1912,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>MD-GGP4-prepreg[0/±45/0]</t>
+          <t>MD-PPG1200-VE4[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -1989,7 +1921,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>MD-HHInjected Short Carbon fiber</t>
+          <t>MD-PPG1200-VE5[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -1998,7 +1930,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>MD-Hybrid CG-VE[(0)2/(0)2C/0/(0)2C/(0)2]</t>
+          <t>MD-PPG1200-VE6[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -2007,7 +1939,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGB-prepreg[(0)2C/±45/(0)2C)</t>
+          <t>MD-P[(0/±45)/M/0/M/(±45/0)]</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -2016,7 +1948,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGB3-prepreg[(±45G)/(0)3C/(±45G)]</t>
+          <t>MD-QQ1-EP2-S[(±45)/(0)2]S</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -2025,7 +1957,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGD4-VE2[(±45G)/(0)3C/(±45G)]</t>
+          <t>MD-QQ1-EP2-S[(±45)/(90)2]S</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -2034,7 +1966,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGD4E-EP3[(±45G)/(0)3C/(±45G)]</t>
+          <t>MD-QQ2-EP2-S[(±45)/0/(±45)]S</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -2043,7 +1975,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>MD-Hybrid JJ-VE2[(±45)/(0)3C/±45)]</t>
+          <t>MD-QQ4-EP2-S[(±45)/0/(+45)]S</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
@@ -2052,227 +1984,11 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>MD-L1200-EP5-D(±45/(0)2)S</t>
+          <t>MD-QQ4M-EP3-S[(±45)/0/(+45)]S</t>
         </is>
       </c>
       <c r="B133" t="inlineStr"/>
       <c r="C133" t="inlineStr"/>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>MD-L1400BTW-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" t="inlineStr"/>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>MD-L1400T-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr"/>
-      <c r="C135" t="inlineStr"/>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>MD-L1400TCS-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>MD-L1400TCU-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr"/>
-      <c r="C137" t="inlineStr"/>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>MD-L1400Thru-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr"/>
-      <c r="C138" t="inlineStr"/>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>MD-L2400-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>MD-LT1200-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr"/>
-      <c r="C140" t="inlineStr"/>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>MD-LT1200G50-EP5-D(±45/(0)2)S</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr"/>
-      <c r="C141" t="inlineStr"/>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>MD-P2B[±45/(0)4C]S</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr"/>
-      <c r="C142" t="inlineStr"/>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>MD-P2B[±45/(90)4C]S</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr"/>
-      <c r="C143" t="inlineStr"/>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>MD-P2C[(±45)/(0)4]S</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr"/>
-      <c r="C144" t="inlineStr"/>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>MD-PPG1200-EP1[(±45)2/(0)2]S</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr"/>
-      <c r="C145" t="inlineStr"/>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>MD-PPG1200-UP5[(±45)2/(0)2]S</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr"/>
-      <c r="C146" t="inlineStr"/>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>MD-PPG1200-VE4[(±45)2/(0)2]S</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr"/>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>MD-PPG1200-VE5[(±45)2/(0)2]S</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr"/>
-      <c r="C148" t="inlineStr"/>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>MD-PPG1200-VE6[(±45)2/(0)2]S</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr"/>
-      <c r="C149" t="inlineStr"/>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>MD-P[(0/±45)/M/0/M/(±45/0)]</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>MD-QQ1-EP2-S[(±45)/(0)2]S</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr"/>
-      <c r="C151" t="inlineStr"/>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>MD-QQ1-EP2-S[(±45)/(90)2]S</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr"/>
-      <c r="C152" t="inlineStr"/>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>MD-QQ2-EP2-S[(±45)/0/(±45)]S</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr"/>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>MD-QQ4-EP2-S[(±45)/0/(+45)]S</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr"/>
-      <c r="C154" t="inlineStr"/>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>MD-QQ4M-EP3-S[(±45)/0/(+45)]S</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr"/>
-      <c r="C155" t="inlineStr"/>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>MD-SLA-UP3-V(±45/0/±45/0/±45)</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr"/>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>MD-SLB-UP3-V(±45/0/±45/0/±45)</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr"/>
-      <c r="C157" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Update better config loading.
</commit_message>
<xml_diff>
--- a/output/material_split.xlsx
+++ b/output/material_split.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -946,7 +946,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EP1 Neat Resin Neat Resin</t>
+          <t>LCCF-K20[0]5</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LCCF-K20[0]5</t>
+          <t>LCCF-T20[0]5</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -980,7 +980,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LCCF-T20[0]5</t>
+          <t>MD-10D155-UP2[±10]3</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -997,7 +997,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MD-10D155-UP2[±10]3</t>
+          <t>MD-20D155-UP2[±20]3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1014,7 +1014,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MD-20D155-UP2[±20]3</t>
+          <t>MD-30D155-UP2[±30]3</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1031,7 +1031,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MD-30D155-UP2[±30]3</t>
+          <t>MD-40D155-UP2[±40]3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MD-40D155-UP2[±40]3</t>
+          <t>MD-45D155-UP2[±45]3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1065,7 +1065,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MD-45D155-UP2[±45]3</t>
+          <t>MD-45D155P2-UP4[±45]3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1082,7 +1082,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MD-45D155P2-UP4[±45]3</t>
+          <t>MD-45D155V-VE[±45]3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1099,7 +1099,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MD-45D155V-VE[±45]3</t>
+          <t>MD-50D155-UP2[±50]3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1116,7 +1116,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>MD-50D155-UP2[±50]3</t>
+          <t>MD-60D155-UP2[±60]3</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1133,7 +1133,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MD-60D155-UP2[±60]3</t>
+          <t>MD-70D155-UP2[±70]3</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1150,7 +1150,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MD-70D155-UP2[±70]3</t>
+          <t>MD-80D155-UP2[±80]3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1167,7 +1167,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MD-80D155-UP2[±80]3</t>
+          <t>MD-90D155-UP2[90]6</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1184,7 +1184,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MD-90D155-UP2[90]6</t>
+          <t>MD-BB-UP2[±45/(0)2/+45]S</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1201,7 +1201,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MD-BB-UP2[±45/(0)2/+45]S</t>
+          <t>MD-BB-UP2[±45/(90)2/+45]S</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1210,7 +1210,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MD-BB-UP2[±45/(90)2/+45]S</t>
+          <t>MD-CC-UP2[±45/(0)2/+45]S</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1219,7 +1219,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MD-CC-UP2[±45/(0)2/+45]S</t>
+          <t>MD-CC2-UP2[±45/(0)3/+45]S</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1228,7 +1228,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MD-CC2-UP2[±45/(0)3/+45]S</t>
+          <t>MD-CC3-UP2[0/±45/(0)2/+45]S</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1237,7 +1237,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MD-CC3-UP2[0/±45/(0)2/+45]S</t>
+          <t>MD-CYC[(±45)2/(0)10]S</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1246,7 +1246,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>MD-CYC[(±45)2/(0)10]S</t>
+          <t>MD-DD-UP2[0/±45/(0)3/±45/0]</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1255,7 +1255,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>MD-DD-UP2[0/±45/(0)3/±45/0]</t>
+          <t>MD-DD10-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1264,7 +1264,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MD-DD10-UP2[0/±45/0]S</t>
+          <t>MD-DD11-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1273,7 +1273,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>MD-DD11-UP2[0/±45/0]S</t>
+          <t>MD-DD11-UP2[90/±45/90]S</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1282,7 +1282,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>MD-DD11-UP2[90/±45/90]S</t>
+          <t>MD-DD11E3-EP3[0/±45/0]S</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1291,7 +1291,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>MD-DD11E3-EP3[0/±45/0]S</t>
+          <t>MD-DD12-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1300,7 +1300,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MD-DD12-UP2[0/±45/0]S</t>
+          <t>MD-DD13-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1309,7 +1309,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MD-DD13-UP2[0/±45/0]S</t>
+          <t>MD-DD14-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1318,7 +1318,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MD-DD14-UP2[0/±45/0]S</t>
+          <t>MD-DD18-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1327,7 +1327,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MD-DD18-UP2[0/±45/0]S</t>
+          <t>MD-DD18A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1336,7 +1336,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MD-DD18A-UP2[0/±45/0]S</t>
+          <t>MD-DD19-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1345,7 +1345,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MD-DD19-UP2[0/±45/0]S</t>
+          <t>MD-DD19A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1354,7 +1354,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>MD-DD19A-UP2[0/±45/0]S</t>
+          <t>MD-DD19A-UP2[90/±45/90]S</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1363,7 +1363,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MD-DD19A-UP2[90/±45/90]S</t>
+          <t>MD-DD19B-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1372,7 +1372,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>MD-DD19B-UP2[0/±45/0]S</t>
+          <t>MD-DD2-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1381,7 +1381,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MD-DD2-UP2[0/±45/0]S</t>
+          <t>MD-DD20-UP2[(0)2/±45/0]S</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1390,7 +1390,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MD-DD20-UP2[(0)2/±45/0]S</t>
+          <t>MD-DD20A-UP2[(0)2/±45/0]S</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1399,7 +1399,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MD-DD20A-UP2[(0)2/±45/0]S</t>
+          <t>MD-DD22-UP2[(0)2/±45/0]S</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1408,7 +1408,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MD-DD22-UP2[(0)2/±45/0]S</t>
+          <t>MD-DD24-UP2[0/±45/(0)3/±45/0]</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -1417,7 +1417,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MD-DD24-UP2[0/±45/(0)3/±45/0]</t>
+          <t>MD-DD25-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1426,7 +1426,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MD-DD25-UP2[0/±45/0]S</t>
+          <t>MD-DD25A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -1435,7 +1435,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>MD-DD25A-UP2[0/±45/0]S</t>
+          <t>MD-DD25B-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1444,7 +1444,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MD-DD25B-UP2[0/±45/0]S</t>
+          <t>MD-DD26-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -1453,7 +1453,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MD-DD26-UP2[0/±45/0]S</t>
+          <t>MD-DD2A-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -1462,7 +1462,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>MD-DD2A-UP2[0/±45/0]S</t>
+          <t>MD-DD4-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -1471,7 +1471,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MD-DD4-UP2[0/±45/0]S</t>
+          <t>MD-DD5-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -1480,7 +1480,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MD-DD5-UP2[0/±45/0]S</t>
+          <t>MD-DD5CYC-T[0/±45/0]S</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -1489,7 +1489,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>MD-DD5CYC-T[0/±45/0]S</t>
+          <t>MD-DD5E-Epon9410[0/±45/0]S</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -1498,7 +1498,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>MD-DD5E-Epon9410[0/±45/0]S</t>
+          <t>MD-DD5E3-EP3[0/±45/0]S</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -1507,7 +1507,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>MD-DD5E3-EP3[0/±45/0]S</t>
+          <t>MD-DD5P-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -1516,7 +1516,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>MD-DD5P-UP2[0/±45/0]S</t>
+          <t>MD-DD5P-UP2[90/±45/90]S</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -1525,7 +1525,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>MD-DD5P-UP2[90/±45/90]S</t>
+          <t>MD-DD5V-VE1[0/±45/0]S</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -1534,7 +1534,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>MD-DD5V-VE1[0/±45/0]S</t>
+          <t>MD-DD5V2-VE2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -1543,7 +1543,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>MD-DD5V2-VE2[0/±45/0]S</t>
+          <t>MD-DD5V3-Dion9800[0/±45/0]S</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -1552,7 +1552,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>MD-DD5V3-Dion9800[0/±45/0]S</t>
+          <t>MD-DD6-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -1561,7 +1561,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>MD-DD6-UP2[0/±45/0]S</t>
+          <t>MD-DD7-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -1570,7 +1570,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>MD-DD7-UP2[0/±45/0]S</t>
+          <t>MD-DD8-UP2[0/±45/0]S</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -1579,7 +1579,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>MD-DD8-UP2[0/±45/0]S</t>
+          <t>MD-EEAP[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -1588,7 +1588,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>MD-EEAP[M/±45/0)S]</t>
+          <t>MD-EEAV[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -1597,7 +1597,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>MD-EEAV[M/±45/0)S]</t>
+          <t>MD-EEBP[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -1606,7 +1606,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>MD-EEBP[M/±45/0)S]</t>
+          <t>MD-EECP[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -1615,7 +1615,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>MD-EECP[M/±45/0)S]</t>
+          <t>MD-EE[M/±45/0)S]</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -1624,7 +1624,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>MD-EE[M/±45/0)S]</t>
+          <t>MD-ELT5500-EP4[±45/0/±45/0/±45]</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -1633,7 +1633,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>MD-ELT5500-EP4[±45/0/±45/0/±45]</t>
+          <t>MD-ELT5500-VE3[±45/0/±45/0/±45]</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -1642,7 +1642,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>MD-ELT5500-VE3[±45/0/±45/0/±45]</t>
+          <t>MD-FFA-UP2[±45/0/0/±45]S</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -1651,7 +1651,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>MD-FFA-UP2[±45/0/0/±45]S</t>
+          <t>MD-FFB-UP2[0/±45/0/±45/0]S</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -1660,7 +1660,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>MD-FFB-UP2[0/±45/0/±45/0]S</t>
+          <t>MD-FFC-UP2[0/±45/±45/0]S</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -1669,7 +1669,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>MD-FFC-UP2[0/±45/±45/0]S</t>
+          <t>MD-FFD-UP2[0/0/±45/±45]S</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -1678,7 +1678,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>MD-FFD-UP2[0/0/±45/±45]S</t>
+          <t>MD-FFF-UP2[±45/±45/0/0]S</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -1687,7 +1687,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>MD-FFF-UP2[±45/±45/0/0]S</t>
+          <t>MD-GG-UP2[(0)2/±45/(0)2]</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -1696,7 +1696,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>MD-GG-UP2[(0)2/±45/(0)2]</t>
+          <t>MD-GGP2-prepreg[0/±45/0]</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -1705,7 +1705,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>MD-GGP2-prepreg[0/±45/0]</t>
+          <t>MD-GGP4-prepreg[0/±45/0]</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -1714,7 +1714,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>MD-GGP4-prepreg[0/±45/0]</t>
+          <t>MD-HHInjected Short Carbon fiber</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -1723,7 +1723,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>MD-HHInjected Short Carbon fiber</t>
+          <t>MD-Hybrid CG-VE[(0)2/(0)2C/0/(0)2C/(0)2]</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -1732,7 +1732,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>MD-Hybrid CG-VE[(0)2/(0)2C/0/(0)2C/(0)2]</t>
+          <t>MD-Hybrid CGB-prepreg[(0)2C/±45/(0)2C)</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -1741,7 +1741,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGB-prepreg[(0)2C/±45/(0)2C)</t>
+          <t>MD-Hybrid CGB3-prepreg[(±45G)/(0)3C/(±45G)]</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -1750,7 +1750,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGB3-prepreg[(±45G)/(0)3C/(±45G)]</t>
+          <t>MD-Hybrid CGD4-VE2[(±45G)/(0)3C/(±45G)]</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -1759,7 +1759,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGD4-VE2[(±45G)/(0)3C/(±45G)]</t>
+          <t>MD-Hybrid CGD4E-EP3[(±45G)/(0)3C/(±45G)]</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -1768,7 +1768,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>MD-Hybrid CGD4E-EP3[(±45G)/(0)3C/(±45G)]</t>
+          <t>MD-Hybrid JJ-VE2[(±45)/(0)3C/±45)]</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -1777,7 +1777,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>MD-Hybrid JJ-VE2[(±45)/(0)3C/±45)]</t>
+          <t>MD-L1200-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -1786,7 +1786,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>MD-L1200-EP5-D(±45/(0)2)S</t>
+          <t>MD-L1400BTW-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -1795,7 +1795,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>MD-L1400BTW-EP5-D(±45/(0)2)S</t>
+          <t>MD-L1400T-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -1804,7 +1804,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>MD-L1400T-EP5-D(±45/(0)2)S</t>
+          <t>MD-L1400TCS-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -1813,7 +1813,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>MD-L1400TCS-EP5-D(±45/(0)2)S</t>
+          <t>MD-L1400TCU-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -1822,7 +1822,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>MD-L1400TCU-EP5-D(±45/(0)2)S</t>
+          <t>MD-L1400Thru-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -1831,7 +1831,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>MD-L1400Thru-EP5-D(±45/(0)2)S</t>
+          <t>MD-L2400-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -1840,7 +1840,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>MD-L2400-EP5-D(±45/(0)2)S</t>
+          <t>MD-LT1200-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -1849,7 +1849,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>MD-LT1200-EP5-D(±45/(0)2)S</t>
+          <t>MD-LT1200G50-EP5-D(±45/(0)2)S</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -1858,7 +1858,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>MD-LT1200G50-EP5-D(±45/(0)2)S</t>
+          <t>MD-P2B[±45/(0)4C]S</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -1867,7 +1867,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>MD-P2B[±45/(0)4C]S</t>
+          <t>MD-P2B[±45/(90)4C]S</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -1876,7 +1876,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>MD-P2B[±45/(90)4C]S</t>
+          <t>MD-P2C[(±45)/(0)4]S</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -1885,7 +1885,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>MD-P2C[(±45)/(0)4]S</t>
+          <t>MD-PPG1200-EP1[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -1894,7 +1894,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>MD-PPG1200-EP1[(±45)2/(0)2]S</t>
+          <t>MD-PPG1200-UP5[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -1903,7 +1903,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>MD-PPG1200-UP5[(±45)2/(0)2]S</t>
+          <t>MD-PPG1200-VE4[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>MD-PPG1200-VE4[(±45)2/(0)2]S</t>
+          <t>MD-PPG1200-VE5[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -1921,7 +1921,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>MD-PPG1200-VE5[(±45)2/(0)2]S</t>
+          <t>MD-PPG1200-VE6[(±45)2/(0)2]S</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -1930,7 +1930,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>MD-PPG1200-VE6[(±45)2/(0)2]S</t>
+          <t>MD-P[(0/±45)/M/0/M/(±45/0)]</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -1939,7 +1939,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>MD-P[(0/±45)/M/0/M/(±45/0)]</t>
+          <t>MD-QQ1-EP2-S[(±45)/(0)2]S</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -1948,7 +1948,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>MD-QQ1-EP2-S[(±45)/(0)2]S</t>
+          <t>MD-QQ1-EP2-S[(±45)/(90)2]S</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -1957,7 +1957,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>MD-QQ1-EP2-S[(±45)/(90)2]S</t>
+          <t>MD-QQ2-EP2-S[(±45)/0/(±45)]S</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -1966,7 +1966,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>MD-QQ2-EP2-S[(±45)/0/(±45)]S</t>
+          <t>MD-QQ4-EP2-S[(±45)/0/(+45)]S</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -1975,20 +1975,11 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>MD-QQ4-EP2-S[(±45)/0/(+45)]S</t>
+          <t>MD-QQ4M-EP3-S[(±45)/0/(+45)]S</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
       <c r="C132" t="inlineStr"/>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>MD-QQ4M-EP3-S[(±45)/0/(+45)]S</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>